<commit_message>
alterações no cadastro para serem corrigidas futuramente
</commit_message>
<xml_diff>
--- a/excel/ExcelAppium.xlsx
+++ b/excel/ExcelAppium.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emerson.prado\eclipse-toolsqa\workspace-appium\AOS_Appium_TDD\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46145A6B-2749-4298-9A95-24C77419E1E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD109D8-C303-47F4-BB42-DDBB2C937415}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="11160" activeTab="1" xr2:uid="{C2A49874-6AB6-4516-A2F6-1E9421577EFB}"/>
   </bookViews>
@@ -108,10 +108,10 @@
     <t>06293110</t>
   </si>
   <si>
-    <t>pradov1027</t>
-  </si>
-  <si>
     <t>Avenida dos Remedios</t>
+  </si>
+  <si>
+    <t>pradov1033</t>
   </si>
 </sst>
 </file>
@@ -525,7 +525,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,7 +573,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>16</v>
@@ -594,7 +594,7 @@
         <v>21</v>
       </c>
       <c r="H2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I2" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
refatoração e ajustes do tdd
</commit_message>
<xml_diff>
--- a/excel/ExcelAppium.xlsx
+++ b/excel/ExcelAppium.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emerson.prado\eclipse-toolsqa\workspace-appium\AOS_Appium_TDD\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21841E9B-7A60-4E80-9645-C42467DB52A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703C3935-E63F-4978-B933-25DCFA94FEDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24315" yWindow="2910" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{C2A49874-6AB6-4516-A2F6-1E9421577EFB}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="11160" activeTab="1" xr2:uid="{C2A49874-6AB6-4516-A2F6-1E9421577EFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Pesquisa" sheetId="1" r:id="rId1"/>
@@ -111,7 +111,7 @@
     <t>Avenida dos Remedios</t>
   </si>
   <si>
-    <t>pradov1051</t>
+    <t>pradov1057</t>
   </si>
 </sst>
 </file>
@@ -525,7 +525,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>